<commit_message>
Hide augment affixes from search
</commit_message>
<xml_diff>
--- a/data-builder/augments.xlsx
+++ b/data-builder/augments.xlsx
@@ -687,9 +687,6 @@
     <t>Illusion Focus</t>
   </si>
   <si>
-    <t>Necromany Focus</t>
-  </si>
-  <si>
     <t>Abjuration Focus</t>
   </si>
   <si>
@@ -703,6 +700,9 @@
   </si>
   <si>
     <t>Augment</t>
+  </si>
+  <si>
+    <t>Necromancy Focus</t>
   </si>
 </sst>
 </file>
@@ -1060,8 +1060,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42:E48"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1659,7 +1659,7 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1673,7 +1673,7 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1681,13 +1681,13 @@
         <v>16</v>
       </c>
       <c r="C44" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1695,13 +1695,13 @@
         <v>16</v>
       </c>
       <c r="C45" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D45">
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1709,13 +1709,13 @@
         <v>16</v>
       </c>
       <c r="C46" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D46">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1723,13 +1723,13 @@
         <v>16</v>
       </c>
       <c r="C47" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1737,13 +1737,13 @@
         <v>16</v>
       </c>
       <c r="C48" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1981,7 +1981,7 @@
         <v>2</v>
       </c>
       <c r="E65" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -1995,7 +1995,7 @@
         <v>2</v>
       </c>
       <c r="E66" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -2003,13 +2003,13 @@
         <v>16</v>
       </c>
       <c r="C67" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="D67">
         <v>2</v>
       </c>
       <c r="E67" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -2017,13 +2017,13 @@
         <v>16</v>
       </c>
       <c r="C68" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D68">
         <v>2</v>
       </c>
       <c r="E68" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -2031,13 +2031,13 @@
         <v>16</v>
       </c>
       <c r="C69" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D69">
         <v>2</v>
       </c>
       <c r="E69" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -2045,13 +2045,13 @@
         <v>16</v>
       </c>
       <c r="C70" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D70">
         <v>2</v>
       </c>
       <c r="E70" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -2059,13 +2059,13 @@
         <v>16</v>
       </c>
       <c r="C71" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D71">
         <v>2</v>
       </c>
       <c r="E71" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Pick up fixes to slavers and augments, plus wiki update
</commit_message>
<xml_diff>
--- a/data-builder/augments.xlsx
+++ b/data-builder/augments.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47E8E6B-FEEC-49A6-8250-7788A64FEC48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9675" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Yellow" sheetId="6" r:id="rId1"/>
@@ -28,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="112">
   <si>
     <t>Minimum Level</t>
   </si>
@@ -222,24 +228,9 @@
     <t>Fire Damage</t>
   </si>
   <si>
-    <t>1d2</t>
-  </si>
-  <si>
-    <t>1d3</t>
-  </si>
-  <si>
-    <t>1d4</t>
-  </si>
-  <si>
     <t>1d6</t>
   </si>
   <si>
-    <t>1d8</t>
-  </si>
-  <si>
-    <t>1d10</t>
-  </si>
-  <si>
     <t>2d6</t>
   </si>
   <si>
@@ -361,12 +352,30 @@
   </si>
   <si>
     <t>bool</t>
+  </si>
+  <si>
+    <t>4d6</t>
+  </si>
+  <si>
+    <t>3d6</t>
+  </si>
+  <si>
+    <t>5d6</t>
+  </si>
+  <si>
+    <t>6d6</t>
+  </si>
+  <si>
+    <t>7d6</t>
+  </si>
+  <si>
+    <t>8d6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -715,18 +724,20 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -741,7 +752,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
         <v>45</v>
@@ -831,7 +842,7 @@
         <v>49</v>
       </c>
       <c r="D7" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
         <v>57</v>
@@ -971,7 +982,7 @@
         <v>49</v>
       </c>
       <c r="D17" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E17" t="s">
         <v>57</v>
@@ -1111,7 +1122,7 @@
         <v>49</v>
       </c>
       <c r="D27" s="5">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E27" t="s">
         <v>57</v>
@@ -1237,7 +1248,7 @@
         <v>49</v>
       </c>
       <c r="D36" s="5">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E36" t="s">
         <v>57</v>
@@ -1318,13 +1329,13 @@
         <v>16</v>
       </c>
       <c r="C42" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D42" s="5">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1332,13 +1343,13 @@
         <v>16</v>
       </c>
       <c r="C43" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D43" s="5">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1346,13 +1357,13 @@
         <v>16</v>
       </c>
       <c r="C44" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D44" s="5">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1360,13 +1371,13 @@
         <v>16</v>
       </c>
       <c r="C45" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D45" s="5">
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1374,13 +1385,13 @@
         <v>16</v>
       </c>
       <c r="C46" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D46" s="5">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1388,13 +1399,13 @@
         <v>16</v>
       </c>
       <c r="C47" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D47" s="5">
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1402,13 +1413,13 @@
         <v>16</v>
       </c>
       <c r="C48" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D48" s="5">
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1447,7 +1458,7 @@
         <v>49</v>
       </c>
       <c r="D51" s="5">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E51" t="s">
         <v>57</v>
@@ -1640,13 +1651,13 @@
         <v>24</v>
       </c>
       <c r="C65" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D65" s="5">
         <v>2</v>
       </c>
       <c r="E65" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -1654,13 +1665,13 @@
         <v>24</v>
       </c>
       <c r="C66" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D66" s="5">
         <v>2</v>
       </c>
       <c r="E66" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -1668,13 +1679,13 @@
         <v>24</v>
       </c>
       <c r="C67" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D67" s="5">
         <v>2</v>
       </c>
       <c r="E67" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -1682,13 +1693,13 @@
         <v>24</v>
       </c>
       <c r="C68" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D68" s="5">
         <v>2</v>
       </c>
       <c r="E68" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -1696,13 +1707,13 @@
         <v>24</v>
       </c>
       <c r="C69" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D69" s="5">
         <v>2</v>
       </c>
       <c r="E69" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -1710,13 +1721,13 @@
         <v>24</v>
       </c>
       <c r="C70" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D70" s="5">
         <v>2</v>
       </c>
       <c r="E70" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -1724,13 +1735,13 @@
         <v>24</v>
       </c>
       <c r="C71" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D71" s="5">
         <v>2</v>
       </c>
       <c r="E71" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1889,18 +1900,18 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E76"/>
+  <autoFilter ref="A1:E76" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1976,7 +1987,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D5" s="2">
         <v>2</v>
@@ -2007,7 +2018,7 @@
         <v>58</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E7" t="s">
         <v>57</v>
@@ -2021,7 +2032,7 @@
         <v>53</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" t="s">
         <v>57</v>
@@ -2035,7 +2046,7 @@
         <v>54</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9" t="s">
         <v>57</v>
@@ -2049,7 +2060,7 @@
         <v>55</v>
       </c>
       <c r="D10" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E10" t="s">
         <v>57</v>
@@ -2060,7 +2071,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D11" s="2">
         <v>4</v>
@@ -2091,7 +2102,7 @@
         <v>58</v>
       </c>
       <c r="D13">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
         <v>57</v>
@@ -2105,7 +2116,7 @@
         <v>53</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E14" t="s">
         <v>57</v>
@@ -2119,7 +2130,7 @@
         <v>54</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E15" t="s">
         <v>57</v>
@@ -2133,7 +2144,7 @@
         <v>55</v>
       </c>
       <c r="D16" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E16" t="s">
         <v>57</v>
@@ -2144,7 +2155,7 @@
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D17" s="2">
         <v>6</v>
@@ -2175,7 +2186,7 @@
         <v>58</v>
       </c>
       <c r="D19">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E19" t="s">
         <v>57</v>
@@ -2189,7 +2200,7 @@
         <v>53</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E20" t="s">
         <v>57</v>
@@ -2203,7 +2214,7 @@
         <v>54</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E21" t="s">
         <v>57</v>
@@ -2217,7 +2228,7 @@
         <v>55</v>
       </c>
       <c r="D22" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E22" t="s">
         <v>57</v>
@@ -2228,7 +2239,7 @@
         <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D23" s="2">
         <v>8</v>
@@ -2259,7 +2270,7 @@
         <v>58</v>
       </c>
       <c r="D25">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E25" t="s">
         <v>57</v>
@@ -2273,7 +2284,7 @@
         <v>53</v>
       </c>
       <c r="D26">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E26" t="s">
         <v>57</v>
@@ -2287,7 +2298,7 @@
         <v>54</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E27" t="s">
         <v>57</v>
@@ -2301,7 +2312,7 @@
         <v>55</v>
       </c>
       <c r="D28" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E28" t="s">
         <v>57</v>
@@ -2312,7 +2323,7 @@
         <v>16</v>
       </c>
       <c r="C29" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D29" s="2">
         <v>10</v>
@@ -2343,7 +2354,7 @@
         <v>53</v>
       </c>
       <c r="D31">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E31" t="s">
         <v>57</v>
@@ -2357,7 +2368,7 @@
         <v>54</v>
       </c>
       <c r="D32">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E32" t="s">
         <v>57</v>
@@ -2371,7 +2382,7 @@
         <v>55</v>
       </c>
       <c r="D33" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E33" t="s">
         <v>57</v>
@@ -2382,7 +2393,7 @@
         <v>20</v>
       </c>
       <c r="C34" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D34" s="2">
         <v>12</v>
@@ -2413,7 +2424,7 @@
         <v>58</v>
       </c>
       <c r="D36">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E36" t="s">
         <v>57</v>
@@ -2427,7 +2438,7 @@
         <v>53</v>
       </c>
       <c r="D37">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E37" t="s">
         <v>57</v>
@@ -2441,7 +2452,7 @@
         <v>54</v>
       </c>
       <c r="D38">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E38" t="s">
         <v>57</v>
@@ -2455,7 +2466,7 @@
         <v>55</v>
       </c>
       <c r="D39" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E39" t="s">
         <v>57</v>
@@ -2466,7 +2477,7 @@
         <v>24</v>
       </c>
       <c r="C40" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D40" s="2">
         <v>14</v>
@@ -2483,7 +2494,7 @@
         <v>58</v>
       </c>
       <c r="D41">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E41" t="s">
         <v>57</v>
@@ -2497,7 +2508,7 @@
         <v>53</v>
       </c>
       <c r="D42">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E42" t="s">
         <v>57</v>
@@ -2511,7 +2522,7 @@
         <v>54</v>
       </c>
       <c r="D43">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E43" t="s">
         <v>57</v>
@@ -2525,7 +2536,7 @@
         <v>55</v>
       </c>
       <c r="D44" s="2">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E44" t="s">
         <v>57</v>
@@ -2536,7 +2547,7 @@
         <v>28</v>
       </c>
       <c r="C45" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D45" s="2">
         <v>16</v>
@@ -2553,7 +2564,7 @@
         <v>58</v>
       </c>
       <c r="D46">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E46" t="s">
         <v>57</v>
@@ -2564,7 +2575,7 @@
         <v>12</v>
       </c>
       <c r="C47" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D47" s="5">
         <v>5</v>
@@ -2578,7 +2589,7 @@
         <v>16</v>
       </c>
       <c r="C48" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D48" s="5">
         <v>10</v>
@@ -2592,7 +2603,7 @@
         <v>20</v>
       </c>
       <c r="C49" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D49" s="5">
         <v>15</v>
@@ -2606,7 +2617,7 @@
         <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D50" s="5">
         <v>1</v>
@@ -2620,7 +2631,7 @@
         <v>20</v>
       </c>
       <c r="C51" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D51" s="5">
         <v>2</v>
@@ -2630,18 +2641,18 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E46"/>
+  <autoFilter ref="A1:E46" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="D120" sqref="D120"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="F121" sqref="F121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2676,8 +2687,8 @@
       <c r="C2" t="s">
         <v>60</v>
       </c>
-      <c r="D2">
-        <v>1</v>
+      <c r="D2" t="s">
+        <v>64</v>
       </c>
       <c r="E2" t="s">
         <v>57</v>
@@ -2690,8 +2701,8 @@
       <c r="C3" t="s">
         <v>61</v>
       </c>
-      <c r="D3">
-        <v>1</v>
+      <c r="D3" t="s">
+        <v>64</v>
       </c>
       <c r="E3" t="s">
         <v>57</v>
@@ -2704,8 +2715,8 @@
       <c r="C4" t="s">
         <v>62</v>
       </c>
-      <c r="D4">
-        <v>1</v>
+      <c r="D4" t="s">
+        <v>64</v>
       </c>
       <c r="E4" t="s">
         <v>57</v>
@@ -2718,8 +2729,8 @@
       <c r="C5" t="s">
         <v>63</v>
       </c>
-      <c r="D5">
-        <v>1</v>
+      <c r="D5" t="s">
+        <v>64</v>
       </c>
       <c r="E5" t="s">
         <v>57</v>
@@ -2731,13 +2742,13 @@
       </c>
       <c r="B6" s="3"/>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D6">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -2746,13 +2757,13 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D7">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -2761,13 +2772,13 @@
       </c>
       <c r="B8" s="3"/>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D8">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -2776,13 +2787,13 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D9">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -2791,13 +2802,13 @@
       </c>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D10">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -2806,13 +2817,13 @@
       </c>
       <c r="B11" s="3"/>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D11">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -2821,13 +2832,13 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D12">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -2836,13 +2847,13 @@
       </c>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D13">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -2851,13 +2862,13 @@
       </c>
       <c r="B14" s="3"/>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D14">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -2866,13 +2877,13 @@
       </c>
       <c r="B15" s="3"/>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D15">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -2883,7 +2894,7 @@
         <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E16" t="s">
         <v>57</v>
@@ -2897,7 +2908,7 @@
         <v>61</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E17" t="s">
         <v>57</v>
@@ -2911,7 +2922,7 @@
         <v>62</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E18" t="s">
         <v>57</v>
@@ -2925,7 +2936,7 @@
         <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E19" t="s">
         <v>57</v>
@@ -2936,13 +2947,13 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D20">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E20" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -2950,13 +2961,13 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D21">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -2964,13 +2975,13 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D22">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E22" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -2978,13 +2989,13 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D23">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -2992,13 +3003,13 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D24">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E24" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -3006,13 +3017,13 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D25">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E25" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -3020,13 +3031,13 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D26">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E26" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -3034,13 +3045,13 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D27">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E27" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -3048,13 +3059,13 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D28">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E28" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -3062,13 +3073,13 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D29">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E29" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3079,7 +3090,7 @@
         <v>60</v>
       </c>
       <c r="D30" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="E30" t="s">
         <v>57</v>
@@ -3093,7 +3104,7 @@
         <v>61</v>
       </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="E31" t="s">
         <v>57</v>
@@ -3107,7 +3118,7 @@
         <v>62</v>
       </c>
       <c r="D32" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="E32" t="s">
         <v>57</v>
@@ -3121,7 +3132,7 @@
         <v>63</v>
       </c>
       <c r="D33" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="E33" t="s">
         <v>57</v>
@@ -3132,7 +3143,7 @@
         <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -3146,7 +3157,7 @@
         <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -3160,7 +3171,7 @@
         <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -3174,7 +3185,7 @@
         <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -3188,13 +3199,13 @@
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D38">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="E38" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3202,13 +3213,13 @@
         <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D39">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="E39" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3216,13 +3227,13 @@
         <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D40">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="E40" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -3230,13 +3241,13 @@
         <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D41">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="E41" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -3244,13 +3255,13 @@
         <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D42">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="E42" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3258,13 +3269,13 @@
         <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D43">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="E43" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3272,13 +3283,13 @@
         <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D44">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="E44" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3286,13 +3297,13 @@
         <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D45">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="E45" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -3300,13 +3311,13 @@
         <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D46">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="E46" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3314,13 +3325,13 @@
         <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D47">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="E47" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3331,7 +3342,7 @@
         <v>60</v>
       </c>
       <c r="D48" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="E48" t="s">
         <v>57</v>
@@ -3345,7 +3356,7 @@
         <v>61</v>
       </c>
       <c r="D49" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="E49" t="s">
         <v>57</v>
@@ -3359,7 +3370,7 @@
         <v>62</v>
       </c>
       <c r="D50" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="E50" t="s">
         <v>57</v>
@@ -3373,7 +3384,7 @@
         <v>63</v>
       </c>
       <c r="D51" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="E51" t="s">
         <v>57</v>
@@ -3384,7 +3395,7 @@
         <v>12</v>
       </c>
       <c r="C52" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -3398,7 +3409,7 @@
         <v>12</v>
       </c>
       <c r="C53" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -3412,13 +3423,13 @@
         <v>12</v>
       </c>
       <c r="C54" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D54">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="E54" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3426,13 +3437,13 @@
         <v>12</v>
       </c>
       <c r="C55" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D55">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="E55" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -3440,13 +3451,13 @@
         <v>12</v>
       </c>
       <c r="C56" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D56">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="E56" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -3454,13 +3465,13 @@
         <v>12</v>
       </c>
       <c r="C57" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D57">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="E57" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3468,13 +3479,13 @@
         <v>12</v>
       </c>
       <c r="C58" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D58">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="E58" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -3482,13 +3493,13 @@
         <v>12</v>
       </c>
       <c r="C59" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D59">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="E59" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -3496,13 +3507,13 @@
         <v>12</v>
       </c>
       <c r="C60" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D60">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="E60" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3510,13 +3521,13 @@
         <v>12</v>
       </c>
       <c r="C61" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D61">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="E61" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3524,13 +3535,13 @@
         <v>12</v>
       </c>
       <c r="C62" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D62">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="E62" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -3538,13 +3549,13 @@
         <v>12</v>
       </c>
       <c r="C63" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D63">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="E63" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -3555,7 +3566,7 @@
         <v>60</v>
       </c>
       <c r="D64" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="E64" t="s">
         <v>57</v>
@@ -3569,7 +3580,7 @@
         <v>61</v>
       </c>
       <c r="D65" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="E65" t="s">
         <v>57</v>
@@ -3583,7 +3594,7 @@
         <v>62</v>
       </c>
       <c r="D66" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="E66" t="s">
         <v>57</v>
@@ -3597,7 +3608,7 @@
         <v>63</v>
       </c>
       <c r="D67" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="E67" t="s">
         <v>57</v>
@@ -3608,7 +3619,7 @@
         <v>16</v>
       </c>
       <c r="C68" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -3622,7 +3633,7 @@
         <v>16</v>
       </c>
       <c r="C69" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D69">
         <v>1</v>
@@ -3636,13 +3647,13 @@
         <v>16</v>
       </c>
       <c r="C70" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D70">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="E70" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3650,13 +3661,13 @@
         <v>16</v>
       </c>
       <c r="C71" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D71">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="E71" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3664,13 +3675,13 @@
         <v>16</v>
       </c>
       <c r="C72" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D72">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="E72" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3678,13 +3689,13 @@
         <v>16</v>
       </c>
       <c r="C73" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D73">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="E73" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3692,13 +3703,13 @@
         <v>16</v>
       </c>
       <c r="C74" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D74">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="E74" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3706,13 +3717,13 @@
         <v>16</v>
       </c>
       <c r="C75" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D75">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="E75" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3720,13 +3731,13 @@
         <v>16</v>
       </c>
       <c r="C76" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D76">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="E76" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3734,13 +3745,13 @@
         <v>16</v>
       </c>
       <c r="C77" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D77">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="E77" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3748,13 +3759,13 @@
         <v>16</v>
       </c>
       <c r="C78" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D78">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="E78" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3762,13 +3773,13 @@
         <v>16</v>
       </c>
       <c r="C79" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D79">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="E79" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -3779,7 +3790,7 @@
         <v>60</v>
       </c>
       <c r="D80" t="s">
-        <v>68</v>
+        <v>109</v>
       </c>
       <c r="E80" t="s">
         <v>57</v>
@@ -3793,7 +3804,7 @@
         <v>61</v>
       </c>
       <c r="D81" t="s">
-        <v>68</v>
+        <v>109</v>
       </c>
       <c r="E81" t="s">
         <v>57</v>
@@ -3807,7 +3818,7 @@
         <v>62</v>
       </c>
       <c r="D82" t="s">
-        <v>68</v>
+        <v>109</v>
       </c>
       <c r="E82" t="s">
         <v>57</v>
@@ -3821,7 +3832,7 @@
         <v>63</v>
       </c>
       <c r="D83" t="s">
-        <v>68</v>
+        <v>109</v>
       </c>
       <c r="E83" t="s">
         <v>57</v>
@@ -3832,13 +3843,13 @@
         <v>20</v>
       </c>
       <c r="C84" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D84">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="E84" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3846,13 +3857,13 @@
         <v>20</v>
       </c>
       <c r="C85" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D85">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="E85" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3860,13 +3871,13 @@
         <v>20</v>
       </c>
       <c r="C86" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D86">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="E86" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3874,13 +3885,13 @@
         <v>20</v>
       </c>
       <c r="C87" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D87">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="E87" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3888,13 +3899,13 @@
         <v>20</v>
       </c>
       <c r="C88" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D88">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="E88" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -3902,13 +3913,13 @@
         <v>20</v>
       </c>
       <c r="C89" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D89">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="E89" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3916,13 +3927,13 @@
         <v>20</v>
       </c>
       <c r="C90" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D90">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="E90" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3930,13 +3941,13 @@
         <v>20</v>
       </c>
       <c r="C91" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D91">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="E91" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3944,13 +3955,13 @@
         <v>20</v>
       </c>
       <c r="C92" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D92">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="E92" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -3958,13 +3969,13 @@
         <v>20</v>
       </c>
       <c r="C93" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D93">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="E93" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3975,7 +3986,7 @@
         <v>60</v>
       </c>
       <c r="D94" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="E94" t="s">
         <v>57</v>
@@ -3989,7 +4000,7 @@
         <v>61</v>
       </c>
       <c r="D95" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="E95" t="s">
         <v>57</v>
@@ -4003,7 +4014,7 @@
         <v>62</v>
       </c>
       <c r="D96" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="E96" t="s">
         <v>57</v>
@@ -4017,7 +4028,7 @@
         <v>63</v>
       </c>
       <c r="D97" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="E97" t="s">
         <v>57</v>
@@ -4028,13 +4039,13 @@
         <v>24</v>
       </c>
       <c r="C98" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D98">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="E98" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -4042,13 +4053,13 @@
         <v>24</v>
       </c>
       <c r="C99" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D99">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="E99" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -4056,13 +4067,13 @@
         <v>24</v>
       </c>
       <c r="C100" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D100">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="E100" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -4070,13 +4081,13 @@
         <v>24</v>
       </c>
       <c r="C101" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D101">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="E101" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -4084,13 +4095,13 @@
         <v>24</v>
       </c>
       <c r="C102" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D102">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="E102" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -4098,13 +4109,13 @@
         <v>24</v>
       </c>
       <c r="C103" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D103">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="E103" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -4112,13 +4123,13 @@
         <v>24</v>
       </c>
       <c r="C104" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D104">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="E104" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -4126,13 +4137,13 @@
         <v>24</v>
       </c>
       <c r="C105" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D105">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="E105" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -4140,13 +4151,13 @@
         <v>24</v>
       </c>
       <c r="C106" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D106">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="E106" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -4154,13 +4165,13 @@
         <v>24</v>
       </c>
       <c r="C107" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D107">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="E107" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -4171,7 +4182,7 @@
         <v>60</v>
       </c>
       <c r="D108" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="E108" t="s">
         <v>57</v>
@@ -4185,7 +4196,7 @@
         <v>61</v>
       </c>
       <c r="D109" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="E109" t="s">
         <v>57</v>
@@ -4199,7 +4210,7 @@
         <v>62</v>
       </c>
       <c r="D110" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="E110" t="s">
         <v>57</v>
@@ -4213,7 +4224,7 @@
         <v>63</v>
       </c>
       <c r="D111" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="E111" t="s">
         <v>57</v>
@@ -4224,13 +4235,13 @@
         <v>28</v>
       </c>
       <c r="C112" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D112">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E112" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -4238,13 +4249,13 @@
         <v>28</v>
       </c>
       <c r="C113" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D113">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E113" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -4252,13 +4263,13 @@
         <v>28</v>
       </c>
       <c r="C114" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D114">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E114" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -4266,13 +4277,13 @@
         <v>28</v>
       </c>
       <c r="C115" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D115">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E115" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -4280,13 +4291,13 @@
         <v>28</v>
       </c>
       <c r="C116" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D116">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E116" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -4294,13 +4305,13 @@
         <v>28</v>
       </c>
       <c r="C117" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D117">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E117" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -4308,13 +4319,13 @@
         <v>28</v>
       </c>
       <c r="C118" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D118">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E118" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -4322,13 +4333,13 @@
         <v>28</v>
       </c>
       <c r="C119" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D119">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E119" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -4336,13 +4347,13 @@
         <v>28</v>
       </c>
       <c r="C120" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D120">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E120" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -4350,28 +4361,29 @@
         <v>28</v>
       </c>
       <c r="C121" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D121">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E121" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E121"/>
+  <autoFilter ref="A1:E121" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:E217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="E217" sqref="E217"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="J223" sqref="J223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4413,7 +4425,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4430,7 +4442,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4441,7 +4453,7 @@
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D4">
         <v>20</v>
@@ -4455,7 +4467,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -4472,7 +4484,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -4489,7 +4501,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -4506,7 +4518,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -4523,7 +4535,7 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -4540,7 +4552,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
@@ -4566,7 +4578,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4583,7 +4595,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4600,7 +4612,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4617,7 +4629,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4634,7 +4646,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4651,7 +4663,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4662,10 +4674,10 @@
         <v>16</v>
       </c>
       <c r="D17" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4676,10 +4688,10 @@
         <v>16</v>
       </c>
       <c r="D18" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4690,10 +4702,10 @@
         <v>16</v>
       </c>
       <c r="D19" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4704,10 +4716,10 @@
         <v>16</v>
       </c>
       <c r="D20" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4718,10 +4730,10 @@
         <v>16</v>
       </c>
       <c r="D21" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4732,10 +4744,10 @@
         <v>16</v>
       </c>
       <c r="D22" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E22" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4746,10 +4758,10 @@
         <v>16</v>
       </c>
       <c r="D23" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E23" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4760,10 +4772,10 @@
         <v>17</v>
       </c>
       <c r="D24" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4774,10 +4786,10 @@
         <v>17</v>
       </c>
       <c r="D25" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4788,10 +4800,10 @@
         <v>17</v>
       </c>
       <c r="D26" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E26" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4802,10 +4814,10 @@
         <v>17</v>
       </c>
       <c r="D27" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4816,10 +4828,10 @@
         <v>17</v>
       </c>
       <c r="D28" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4830,10 +4842,10 @@
         <v>17</v>
       </c>
       <c r="D29" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E29" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4844,10 +4856,10 @@
         <v>17</v>
       </c>
       <c r="D30" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E30" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4872,7 +4884,7 @@
         <v>14</v>
       </c>
       <c r="D32" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E32" t="s">
         <v>57</v>
@@ -4886,7 +4898,7 @@
         <v>14</v>
       </c>
       <c r="D33" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E33" t="s">
         <v>57</v>
@@ -4900,7 +4912,7 @@
         <v>14</v>
       </c>
       <c r="D34" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E34" t="s">
         <v>57</v>
@@ -4914,7 +4926,7 @@
         <v>14</v>
       </c>
       <c r="D35" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E35" t="s">
         <v>57</v>
@@ -4928,7 +4940,7 @@
         <v>14</v>
       </c>
       <c r="D36" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E36" t="s">
         <v>57</v>
@@ -4942,7 +4954,7 @@
         <v>14</v>
       </c>
       <c r="D37" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E37" t="s">
         <v>57</v>
@@ -4959,7 +4971,7 @@
         <v>2</v>
       </c>
       <c r="E38" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4970,7 +4982,7 @@
         <v>14</v>
       </c>
       <c r="D39" s="2">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E39" t="s">
         <v>57</v>
@@ -4984,10 +4996,10 @@
         <v>18</v>
       </c>
       <c r="D40" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E40" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -4998,10 +5010,10 @@
         <v>18</v>
       </c>
       <c r="D41" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E41" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5012,10 +5024,10 @@
         <v>18</v>
       </c>
       <c r="D42" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E42" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5026,10 +5038,10 @@
         <v>18</v>
       </c>
       <c r="D43" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E43" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5040,10 +5052,10 @@
         <v>18</v>
       </c>
       <c r="D44" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E44" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5054,10 +5066,10 @@
         <v>18</v>
       </c>
       <c r="D45" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E45" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5068,10 +5080,10 @@
         <v>18</v>
       </c>
       <c r="D46" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E46" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5096,7 +5108,7 @@
         <v>11</v>
       </c>
       <c r="D48" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E48" t="s">
         <v>57</v>
@@ -5110,7 +5122,7 @@
         <v>11</v>
       </c>
       <c r="D49" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E49" t="s">
         <v>57</v>
@@ -5124,7 +5136,7 @@
         <v>11</v>
       </c>
       <c r="D50" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E50" t="s">
         <v>57</v>
@@ -5138,7 +5150,7 @@
         <v>11</v>
       </c>
       <c r="D51" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E51" t="s">
         <v>57</v>
@@ -5152,7 +5164,7 @@
         <v>11</v>
       </c>
       <c r="D52" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E52" t="s">
         <v>57</v>
@@ -5166,7 +5178,7 @@
         <v>11</v>
       </c>
       <c r="D53" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E53" t="s">
         <v>57</v>
@@ -5183,7 +5195,7 @@
         <v>2</v>
       </c>
       <c r="E54" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5194,7 +5206,7 @@
         <v>11</v>
       </c>
       <c r="D55" s="2">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E55" t="s">
         <v>57</v>
@@ -5309,7 +5321,7 @@
         <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5334,10 +5346,10 @@
         <v>19</v>
       </c>
       <c r="D65" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E65" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5348,10 +5360,10 @@
         <v>19</v>
       </c>
       <c r="D66" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E66" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5362,10 +5374,10 @@
         <v>19</v>
       </c>
       <c r="D67" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E67" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5376,10 +5388,10 @@
         <v>19</v>
       </c>
       <c r="D68" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E68" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5390,10 +5402,10 @@
         <v>19</v>
       </c>
       <c r="D69" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E69" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5404,10 +5416,10 @@
         <v>19</v>
       </c>
       <c r="D70" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E70" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5418,10 +5430,10 @@
         <v>19</v>
       </c>
       <c r="D71" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E71" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5432,10 +5444,10 @@
         <v>20</v>
       </c>
       <c r="D72" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E72" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5446,10 +5458,10 @@
         <v>20</v>
       </c>
       <c r="D73" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E73" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5460,10 +5472,10 @@
         <v>20</v>
       </c>
       <c r="D74" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E74" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5474,10 +5486,10 @@
         <v>20</v>
       </c>
       <c r="D75" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E75" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5488,10 +5500,10 @@
         <v>20</v>
       </c>
       <c r="D76" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E76" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5502,10 +5514,10 @@
         <v>20</v>
       </c>
       <c r="D77" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E77" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5516,10 +5528,10 @@
         <v>20</v>
       </c>
       <c r="D78" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E78" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5530,10 +5542,10 @@
         <v>21</v>
       </c>
       <c r="D79" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E79" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5544,10 +5556,10 @@
         <v>21</v>
       </c>
       <c r="D80" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E80" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5558,10 +5570,10 @@
         <v>21</v>
       </c>
       <c r="D81" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E81" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5572,10 +5584,10 @@
         <v>21</v>
       </c>
       <c r="D82" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E82" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5586,10 +5598,10 @@
         <v>21</v>
       </c>
       <c r="D83" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E83" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5600,10 +5612,10 @@
         <v>21</v>
       </c>
       <c r="D84" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E84" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5614,10 +5626,10 @@
         <v>21</v>
       </c>
       <c r="D85" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E85" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5628,10 +5640,10 @@
         <v>22</v>
       </c>
       <c r="D86" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E86" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5642,10 +5654,10 @@
         <v>22</v>
       </c>
       <c r="D87" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E87" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5656,10 +5668,10 @@
         <v>22</v>
       </c>
       <c r="D88" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E88" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5670,10 +5682,10 @@
         <v>22</v>
       </c>
       <c r="D89" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E89" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5684,10 +5696,10 @@
         <v>22</v>
       </c>
       <c r="D90" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E90" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5698,10 +5710,10 @@
         <v>22</v>
       </c>
       <c r="D91" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E91" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5712,10 +5724,10 @@
         <v>22</v>
       </c>
       <c r="D92" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E92" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5726,10 +5738,10 @@
         <v>23</v>
       </c>
       <c r="D93" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E93" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5740,10 +5752,10 @@
         <v>23</v>
       </c>
       <c r="D94" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E94" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5754,10 +5766,10 @@
         <v>23</v>
       </c>
       <c r="D95" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E95" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5768,10 +5780,10 @@
         <v>23</v>
       </c>
       <c r="D96" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E96" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5782,10 +5794,10 @@
         <v>23</v>
       </c>
       <c r="D97" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E97" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5796,10 +5808,10 @@
         <v>23</v>
       </c>
       <c r="D98" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E98" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5810,10 +5822,10 @@
         <v>23</v>
       </c>
       <c r="D99" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E99" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5838,7 +5850,7 @@
         <v>12</v>
       </c>
       <c r="D101" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E101" t="s">
         <v>57</v>
@@ -5852,7 +5864,7 @@
         <v>12</v>
       </c>
       <c r="D102" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E102" t="s">
         <v>57</v>
@@ -5866,7 +5878,7 @@
         <v>12</v>
       </c>
       <c r="D103" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E103" t="s">
         <v>57</v>
@@ -5880,7 +5892,7 @@
         <v>12</v>
       </c>
       <c r="D104" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E104" t="s">
         <v>57</v>
@@ -5894,7 +5906,7 @@
         <v>12</v>
       </c>
       <c r="D105" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E105" t="s">
         <v>57</v>
@@ -5908,7 +5920,7 @@
         <v>12</v>
       </c>
       <c r="D106" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E106" t="s">
         <v>57</v>
@@ -5925,7 +5937,7 @@
         <v>2</v>
       </c>
       <c r="E107" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -5936,7 +5948,7 @@
         <v>12</v>
       </c>
       <c r="D108" s="2">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E108" t="s">
         <v>57</v>
@@ -5950,7 +5962,7 @@
         <v>24</v>
       </c>
       <c r="D109" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E109" t="s">
         <v>57</v>
@@ -5964,7 +5976,7 @@
         <v>24</v>
       </c>
       <c r="D110" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E110" t="s">
         <v>57</v>
@@ -5978,7 +5990,7 @@
         <v>24</v>
       </c>
       <c r="D111" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E111" t="s">
         <v>57</v>
@@ -5992,7 +6004,7 @@
         <v>24</v>
       </c>
       <c r="D112" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E112" t="s">
         <v>57</v>
@@ -6006,7 +6018,7 @@
         <v>24</v>
       </c>
       <c r="D113" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E113" t="s">
         <v>57</v>
@@ -6020,7 +6032,7 @@
         <v>24</v>
       </c>
       <c r="D114" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E114" t="s">
         <v>57</v>
@@ -6034,7 +6046,7 @@
         <v>24</v>
       </c>
       <c r="D115" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E115" t="s">
         <v>57</v>
@@ -6048,10 +6060,10 @@
         <v>25</v>
       </c>
       <c r="D116" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E116" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -6062,10 +6074,10 @@
         <v>25</v>
       </c>
       <c r="D117" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E117" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -6076,10 +6088,10 @@
         <v>25</v>
       </c>
       <c r="D118" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E118" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -6090,10 +6102,10 @@
         <v>25</v>
       </c>
       <c r="D119" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E119" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -6104,10 +6116,10 @@
         <v>25</v>
       </c>
       <c r="D120" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E120" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -6118,10 +6130,10 @@
         <v>25</v>
       </c>
       <c r="D121" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E121" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -6132,10 +6144,10 @@
         <v>25</v>
       </c>
       <c r="D122" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E122" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -6146,10 +6158,10 @@
         <v>26</v>
       </c>
       <c r="D123" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E123" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -6160,10 +6172,10 @@
         <v>26</v>
       </c>
       <c r="D124" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E124" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -6174,10 +6186,10 @@
         <v>26</v>
       </c>
       <c r="D125" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E125" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -6188,10 +6200,10 @@
         <v>26</v>
       </c>
       <c r="D126" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E126" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -6202,10 +6214,10 @@
         <v>26</v>
       </c>
       <c r="D127" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E127" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -6216,10 +6228,10 @@
         <v>26</v>
       </c>
       <c r="D128" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E128" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -6230,10 +6242,10 @@
         <v>26</v>
       </c>
       <c r="D129" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E129" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -6244,10 +6256,10 @@
         <v>27</v>
       </c>
       <c r="D130" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E130" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -6258,10 +6270,10 @@
         <v>27</v>
       </c>
       <c r="D131" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E131" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -6272,10 +6284,10 @@
         <v>27</v>
       </c>
       <c r="D132" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E132" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -6286,10 +6298,10 @@
         <v>27</v>
       </c>
       <c r="D133" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E133" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -6300,10 +6312,10 @@
         <v>27</v>
       </c>
       <c r="D134" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E134" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -6314,10 +6326,10 @@
         <v>27</v>
       </c>
       <c r="D135" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E135" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -6328,10 +6340,10 @@
         <v>27</v>
       </c>
       <c r="D136" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E136" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -6342,10 +6354,10 @@
         <v>28</v>
       </c>
       <c r="D137" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E137" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -6356,10 +6368,10 @@
         <v>28</v>
       </c>
       <c r="D138" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E138" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -6370,10 +6382,10 @@
         <v>28</v>
       </c>
       <c r="D139" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E139" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -6384,10 +6396,10 @@
         <v>28</v>
       </c>
       <c r="D140" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E140" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -6398,10 +6410,10 @@
         <v>28</v>
       </c>
       <c r="D141" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E141" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -6412,10 +6424,10 @@
         <v>28</v>
       </c>
       <c r="D142" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E142" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -6426,10 +6438,10 @@
         <v>28</v>
       </c>
       <c r="D143" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E143" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -6440,10 +6452,10 @@
         <v>29</v>
       </c>
       <c r="D144" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E144" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -6454,10 +6466,10 @@
         <v>29</v>
       </c>
       <c r="D145" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E145" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -6468,10 +6480,10 @@
         <v>29</v>
       </c>
       <c r="D146" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E146" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -6482,10 +6494,10 @@
         <v>29</v>
       </c>
       <c r="D147" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E147" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -6496,10 +6508,10 @@
         <v>29</v>
       </c>
       <c r="D148" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E148" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -6510,10 +6522,10 @@
         <v>29</v>
       </c>
       <c r="D149" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E149" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -6524,10 +6536,10 @@
         <v>29</v>
       </c>
       <c r="D150" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E150" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -6538,10 +6550,10 @@
         <v>30</v>
       </c>
       <c r="D151" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E151" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -6552,10 +6564,10 @@
         <v>30</v>
       </c>
       <c r="D152" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E152" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -6566,10 +6578,10 @@
         <v>30</v>
       </c>
       <c r="D153" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E153" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -6580,10 +6592,10 @@
         <v>30</v>
       </c>
       <c r="D154" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E154" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -6594,10 +6606,10 @@
         <v>30</v>
       </c>
       <c r="D155" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E155" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -6608,10 +6620,10 @@
         <v>30</v>
       </c>
       <c r="D156" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E156" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -6622,10 +6634,10 @@
         <v>30</v>
       </c>
       <c r="D157" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E157" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -6636,10 +6648,10 @@
         <v>31</v>
       </c>
       <c r="D158" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E158" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -6650,10 +6662,10 @@
         <v>31</v>
       </c>
       <c r="D159" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E159" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -6664,10 +6676,10 @@
         <v>31</v>
       </c>
       <c r="D160" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E160" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -6678,10 +6690,10 @@
         <v>31</v>
       </c>
       <c r="D161" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E161" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -6692,10 +6704,10 @@
         <v>31</v>
       </c>
       <c r="D162" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E162" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -6706,10 +6718,10 @@
         <v>31</v>
       </c>
       <c r="D163" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E163" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -6720,10 +6732,10 @@
         <v>31</v>
       </c>
       <c r="D164" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E164" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -6734,10 +6746,10 @@
         <v>32</v>
       </c>
       <c r="D165" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E165" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -6748,10 +6760,10 @@
         <v>32</v>
       </c>
       <c r="D166" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E166" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -6762,10 +6774,10 @@
         <v>32</v>
       </c>
       <c r="D167" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E167" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -6776,10 +6788,10 @@
         <v>32</v>
       </c>
       <c r="D168" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E168" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -6790,10 +6802,10 @@
         <v>32</v>
       </c>
       <c r="D169" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E169" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -6804,10 +6816,10 @@
         <v>32</v>
       </c>
       <c r="D170" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E170" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -6818,10 +6830,10 @@
         <v>32</v>
       </c>
       <c r="D171" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E171" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -6832,10 +6844,10 @@
         <v>33</v>
       </c>
       <c r="D172" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E172" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -6846,10 +6858,10 @@
         <v>33</v>
       </c>
       <c r="D173" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E173" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -6860,10 +6872,10 @@
         <v>33</v>
       </c>
       <c r="D174" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E174" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -6874,10 +6886,10 @@
         <v>33</v>
       </c>
       <c r="D175" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E175" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -6888,10 +6900,10 @@
         <v>33</v>
       </c>
       <c r="D176" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E176" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -6902,10 +6914,10 @@
         <v>33</v>
       </c>
       <c r="D177" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E177" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -6916,10 +6928,10 @@
         <v>33</v>
       </c>
       <c r="D178" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E178" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
@@ -6944,7 +6956,7 @@
         <v>9</v>
       </c>
       <c r="D180" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E180" t="s">
         <v>57</v>
@@ -6958,7 +6970,7 @@
         <v>9</v>
       </c>
       <c r="D181" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E181" t="s">
         <v>57</v>
@@ -6972,7 +6984,7 @@
         <v>9</v>
       </c>
       <c r="D182" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E182" t="s">
         <v>57</v>
@@ -6986,7 +6998,7 @@
         <v>9</v>
       </c>
       <c r="D183" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E183" t="s">
         <v>57</v>
@@ -7000,7 +7012,7 @@
         <v>9</v>
       </c>
       <c r="D184" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E184" t="s">
         <v>57</v>
@@ -7014,7 +7026,7 @@
         <v>9</v>
       </c>
       <c r="D185" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E185" t="s">
         <v>57</v>
@@ -7031,7 +7043,7 @@
         <v>2</v>
       </c>
       <c r="E186" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -7042,7 +7054,7 @@
         <v>9</v>
       </c>
       <c r="D187" s="2">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E187" t="s">
         <v>57</v>
@@ -7056,10 +7068,10 @@
         <v>34</v>
       </c>
       <c r="D188" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E188" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -7070,10 +7082,10 @@
         <v>34</v>
       </c>
       <c r="D189" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E189" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -7084,10 +7096,10 @@
         <v>34</v>
       </c>
       <c r="D190" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E190" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -7098,10 +7110,10 @@
         <v>34</v>
       </c>
       <c r="D191" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E191" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -7112,10 +7124,10 @@
         <v>34</v>
       </c>
       <c r="D192" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E192" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -7126,10 +7138,10 @@
         <v>34</v>
       </c>
       <c r="D193" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E193" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -7140,10 +7152,10 @@
         <v>34</v>
       </c>
       <c r="D194" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E194" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -7154,10 +7166,10 @@
         <v>35</v>
       </c>
       <c r="D195" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E195" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -7168,10 +7180,10 @@
         <v>35</v>
       </c>
       <c r="D196" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E196" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -7182,10 +7194,10 @@
         <v>35</v>
       </c>
       <c r="D197" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E197" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -7196,10 +7208,10 @@
         <v>35</v>
       </c>
       <c r="D198" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E198" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -7210,10 +7222,10 @@
         <v>35</v>
       </c>
       <c r="D199" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E199" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -7224,10 +7236,10 @@
         <v>35</v>
       </c>
       <c r="D200" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E200" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -7238,10 +7250,10 @@
         <v>35</v>
       </c>
       <c r="D201" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E201" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -7266,7 +7278,7 @@
         <v>13</v>
       </c>
       <c r="D203" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E203" t="s">
         <v>57</v>
@@ -7280,7 +7292,7 @@
         <v>13</v>
       </c>
       <c r="D204" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E204" t="s">
         <v>57</v>
@@ -7294,7 +7306,7 @@
         <v>13</v>
       </c>
       <c r="D205" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E205" t="s">
         <v>57</v>
@@ -7308,7 +7320,7 @@
         <v>13</v>
       </c>
       <c r="D206" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E206" t="s">
         <v>57</v>
@@ -7322,7 +7334,7 @@
         <v>13</v>
       </c>
       <c r="D207" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E207" t="s">
         <v>57</v>
@@ -7336,7 +7348,7 @@
         <v>13</v>
       </c>
       <c r="D208" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E208" t="s">
         <v>57</v>
@@ -7353,7 +7365,7 @@
         <v>2</v>
       </c>
       <c r="E209" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -7364,7 +7376,7 @@
         <v>13</v>
       </c>
       <c r="D210" s="2">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E210" t="s">
         <v>57</v>
@@ -7381,7 +7393,7 @@
         <v>1</v>
       </c>
       <c r="E211" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -7395,7 +7407,7 @@
         <v>1</v>
       </c>
       <c r="E212" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
@@ -7409,7 +7421,7 @@
         <v>1</v>
       </c>
       <c r="E213" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -7423,7 +7435,7 @@
         <v>1</v>
       </c>
       <c r="E214" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -7437,7 +7449,7 @@
         <v>1</v>
       </c>
       <c r="E215" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
@@ -7451,26 +7463,26 @@
         <v>1</v>
       </c>
       <c r="E216" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D217" s="2">
         <v>1</v>
       </c>
       <c r="E217" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E201">
-    <sortState ref="A2:E216">
+  <autoFilter ref="A1:E201" xr:uid="{00000000-0009-0000-0000-000003000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E216">
       <sortCondition ref="B1:B201"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
augment update -meridian fragment
</commit_message>
<xml_diff>
--- a/data-builder/augments.xlsx
+++ b/data-builder/augments.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Yellow" sheetId="6" r:id="rId1"/>
     <sheet name="Blue" sheetId="5" r:id="rId2"/>
     <sheet name="Red" sheetId="4" r:id="rId3"/>
     <sheet name="Colorless" sheetId="2" r:id="rId4"/>
+    <sheet name="Orange" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Blue!$A$1:$E$46</definedName>
@@ -18,26 +19,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Red!$A$1:$E$121</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Yellow!$A$1:$E$76</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1156" uniqueCount="132">
   <si>
     <t>Minimum Level</t>
   </si>
@@ -421,6 +408,18 @@
   </si>
   <si>
     <t>Heroic Inspiration</t>
+  </si>
+  <si>
+    <t>Orange Augments</t>
+  </si>
+  <si>
+    <t>Meridian Fragment</t>
+  </si>
+  <si>
+    <t>Efficient Maximize</t>
+  </si>
+  <si>
+    <t>On receiving physical damage, gain a stack of Psionic Potency +8</t>
   </si>
 </sst>
 </file>
@@ -490,9 +489,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -798,7 +794,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A70" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -2267,7 +2263,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
@@ -3636,8 +3632,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E123"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="B120" sqref="B120"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5401,9 +5397,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:E219"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="D128" sqref="D128"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8530,4 +8524,67 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update bonus type on Sapphire of Natural Armor augment to be a Natural bonus to AC to match other affixes
</commit_message>
<xml_diff>
--- a/data-builder/augments.xlsx
+++ b/data-builder/augments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E644CA-7796-4CA0-BFFF-D64F4D48B3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED03EE9-B1A8-4545-A57E-EB9B9E7C15AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19500" yWindow="10830" windowWidth="24150" windowHeight="18330" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="32040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Yellow" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="410">
   <si>
     <t>Minimum Level</t>
   </si>
@@ -1275,6 +1275,9 @@
   </si>
   <si>
     <t>Deflection</t>
+  </si>
+  <si>
+    <t>Natural</t>
   </si>
 </sst>
 </file>
@@ -1282,7 +1285,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -1372,10 +1375,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6387,10 +6390,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A164"/>
+      <selection activeCell="E165" sqref="E165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -6434,10 +6438,10 @@
         <v>1</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" hidden="1">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -6451,7 +6455,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" hidden="1">
       <c r="A4" s="10">
         <v>1</v>
       </c>
@@ -6465,7 +6469,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" hidden="1">
       <c r="A5" s="10">
         <v>1</v>
       </c>
@@ -6479,7 +6483,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" hidden="1">
       <c r="A6" s="10">
         <v>1</v>
       </c>
@@ -6493,7 +6497,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" hidden="1">
       <c r="A7" s="10">
         <v>1</v>
       </c>
@@ -6518,10 +6522,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" hidden="1">
       <c r="A9" s="10">
         <v>4</v>
       </c>
@@ -6535,7 +6539,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" hidden="1">
       <c r="A10" s="10">
         <v>4</v>
       </c>
@@ -6549,7 +6553,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" hidden="1">
       <c r="A11" s="10">
         <v>4</v>
       </c>
@@ -6563,7 +6567,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" hidden="1">
       <c r="A12" s="10">
         <v>4</v>
       </c>
@@ -6577,7 +6581,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" hidden="1">
       <c r="A13" s="10">
         <v>4</v>
       </c>
@@ -6602,10 +6606,10 @@
         <v>5</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" hidden="1">
       <c r="A15" s="10">
         <v>8</v>
       </c>
@@ -6619,7 +6623,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" hidden="1">
       <c r="A16" s="10">
         <v>8</v>
       </c>
@@ -6633,7 +6637,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" hidden="1">
       <c r="A17" s="10">
         <v>8</v>
       </c>
@@ -6647,7 +6651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" hidden="1">
       <c r="A18" s="10">
         <v>8</v>
       </c>
@@ -6661,7 +6665,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" hidden="1">
       <c r="A19" s="10">
         <v>8</v>
       </c>
@@ -6686,10 +6690,10 @@
         <v>6</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A21" s="10">
         <v>12</v>
       </c>
@@ -6703,7 +6707,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1">
+    <row r="22" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A22" s="10">
         <v>12</v>
       </c>
@@ -6717,7 +6721,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1">
+    <row r="23" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A23" s="10">
         <v>12</v>
       </c>
@@ -6731,7 +6735,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1">
+    <row r="24" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A24" s="10">
         <v>12</v>
       </c>
@@ -6745,7 +6749,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1">
+    <row r="25" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A25" s="10">
         <v>12</v>
       </c>
@@ -6770,10 +6774,10 @@
         <v>8</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A27" s="10">
         <v>16</v>
       </c>
@@ -6787,7 +6791,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+    <row r="28" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A28" s="10">
         <v>16</v>
       </c>
@@ -6801,7 +6805,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1">
+    <row r="29" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A29" s="10">
         <v>16</v>
       </c>
@@ -6815,7 +6819,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+    <row r="30" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A30" s="10">
         <v>16</v>
       </c>
@@ -6840,10 +6844,10 @@
         <v>9</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A32" s="10">
         <v>20</v>
       </c>
@@ -6857,7 +6861,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1">
+    <row r="33" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A33" s="10">
         <v>20</v>
       </c>
@@ -6871,7 +6875,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1">
+    <row r="34" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A34" s="10">
         <v>20</v>
       </c>
@@ -6885,7 +6889,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1">
+    <row r="35" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A35" s="10">
         <v>20</v>
       </c>
@@ -6899,7 +6903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1">
+    <row r="36" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A36" s="10">
         <v>20</v>
       </c>
@@ -6924,10 +6928,10 @@
         <v>11</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A38" s="10">
         <v>24</v>
       </c>
@@ -6941,7 +6945,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1">
+    <row r="39" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A39" s="10">
         <v>24</v>
       </c>
@@ -6955,7 +6959,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1">
+    <row r="40" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A40" s="10">
         <v>24</v>
       </c>
@@ -6969,7 +6973,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1">
+    <row r="41" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A41" s="10">
         <v>24</v>
       </c>
@@ -6994,10 +6998,10 @@
         <v>12</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A43" s="10">
         <v>28</v>
       </c>
@@ -7011,7 +7015,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1">
+    <row r="44" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A44" s="10">
         <v>28</v>
       </c>
@@ -7025,7 +7029,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1">
+    <row r="45" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A45" s="10">
         <v>28</v>
       </c>
@@ -7039,7 +7043,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1">
+    <row r="46" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A46" s="10">
         <v>28</v>
       </c>
@@ -7053,7 +7057,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1">
+    <row r="47" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A47" s="10">
         <v>12</v>
       </c>
@@ -7067,7 +7071,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1">
+    <row r="48" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A48" s="10">
         <v>16</v>
       </c>
@@ -7081,7 +7085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1">
+    <row r="49" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A49" s="10">
         <v>20</v>
       </c>
@@ -7095,7 +7099,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1">
+    <row r="50" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A50" s="10">
         <v>12</v>
       </c>
@@ -7109,7 +7113,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1">
+    <row r="51" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A51" s="10">
         <v>20</v>
       </c>
@@ -7123,7 +7127,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1">
+    <row r="52" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A52" s="10">
         <v>1</v>
       </c>
@@ -7137,7 +7141,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1">
+    <row r="53" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A53" s="10">
         <v>4</v>
       </c>
@@ -7151,7 +7155,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1">
+    <row r="54" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A54" s="10">
         <v>8</v>
       </c>
@@ -7165,7 +7169,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15.75" customHeight="1">
+    <row r="55" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A55" s="10">
         <v>12</v>
       </c>
@@ -7179,7 +7183,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15.75" customHeight="1">
+    <row r="56" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A56" s="10">
         <v>16</v>
       </c>
@@ -7193,7 +7197,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="15.75" customHeight="1">
+    <row r="57" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A57" s="10">
         <v>20</v>
       </c>
@@ -7207,7 +7211,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15.75" customHeight="1">
+    <row r="58" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A58" s="10">
         <v>24</v>
       </c>
@@ -7221,7 +7225,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15.75" customHeight="1">
+    <row r="59" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A59" s="10">
         <v>28</v>
       </c>
@@ -7235,7 +7239,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="15.75" customHeight="1">
+    <row r="60" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A60" s="10">
         <v>32</v>
       </c>
@@ -7249,7 +7253,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1">
+    <row r="61" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A61" s="10">
         <v>1</v>
       </c>
@@ -7263,7 +7267,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1">
+    <row r="62" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A62" s="10">
         <v>4</v>
       </c>
@@ -7277,7 +7281,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1">
+    <row r="63" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A63" s="10">
         <v>8</v>
       </c>
@@ -7291,7 +7295,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1">
+    <row r="64" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A64" s="10">
         <v>12</v>
       </c>
@@ -7305,7 +7309,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1">
+    <row r="65" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A65" s="10">
         <v>16</v>
       </c>
@@ -7319,7 +7323,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1">
+    <row r="66" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A66" s="10">
         <v>20</v>
       </c>
@@ -7333,7 +7337,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1">
+    <row r="67" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A67" s="10">
         <v>24</v>
       </c>
@@ -7347,7 +7351,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1">
+    <row r="68" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A68" s="10">
         <v>28</v>
       </c>
@@ -7361,7 +7365,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1">
+    <row r="69" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A69" s="10">
         <v>32</v>
       </c>
@@ -7375,7 +7379,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1">
+    <row r="70" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A70" s="10">
         <v>1</v>
       </c>
@@ -7389,7 +7393,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1">
+    <row r="71" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A71" s="10">
         <v>4</v>
       </c>
@@ -7403,7 +7407,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1">
+    <row r="72" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A72" s="10">
         <v>8</v>
       </c>
@@ -7417,7 +7421,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1">
+    <row r="73" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A73" s="10">
         <v>12</v>
       </c>
@@ -7431,7 +7435,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1">
+    <row r="74" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A74" s="10">
         <v>16</v>
       </c>
@@ -7445,7 +7449,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1">
+    <row r="75" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A75" s="10">
         <v>20</v>
       </c>
@@ -7459,7 +7463,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1">
+    <row r="76" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A76" s="10">
         <v>24</v>
       </c>
@@ -7473,7 +7477,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1">
+    <row r="77" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A77" s="10">
         <v>28</v>
       </c>
@@ -7487,7 +7491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1">
+    <row r="78" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A78" s="10">
         <v>32</v>
       </c>
@@ -7501,7 +7505,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1">
+    <row r="79" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A79" s="10">
         <v>1</v>
       </c>
@@ -7515,7 +7519,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1">
+    <row r="80" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A80" s="10">
         <v>4</v>
       </c>
@@ -7529,7 +7533,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1">
+    <row r="81" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A81" s="10">
         <v>8</v>
       </c>
@@ -7543,7 +7547,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1">
+    <row r="82" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A82" s="10">
         <v>12</v>
       </c>
@@ -7557,7 +7561,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1">
+    <row r="83" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A83" s="10">
         <v>16</v>
       </c>
@@ -7571,7 +7575,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="15.75" customHeight="1">
+    <row r="84" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A84" s="10">
         <v>20</v>
       </c>
@@ -7585,7 +7589,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="15.75" customHeight="1">
+    <row r="85" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A85" s="10">
         <v>24</v>
       </c>
@@ -7599,7 +7603,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="15.75" customHeight="1">
+    <row r="86" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A86" s="10">
         <v>28</v>
       </c>
@@ -7613,7 +7617,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="15.75" customHeight="1">
+    <row r="87" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A87" s="10">
         <v>32</v>
       </c>
@@ -7627,7 +7631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="15.75" customHeight="1">
+    <row r="88" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A88" s="10">
         <v>1</v>
       </c>
@@ -7641,7 +7645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="15.75" customHeight="1">
+    <row r="89" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A89" s="10">
         <v>4</v>
       </c>
@@ -7655,7 +7659,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="15.75" customHeight="1">
+    <row r="90" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A90" s="10">
         <v>8</v>
       </c>
@@ -7669,7 +7673,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="15.75" customHeight="1">
+    <row r="91" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A91" s="10">
         <v>12</v>
       </c>
@@ -7683,7 +7687,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="15.75" customHeight="1">
+    <row r="92" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A92" s="10">
         <v>16</v>
       </c>
@@ -7697,7 +7701,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="15.75" customHeight="1">
+    <row r="93" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A93" s="10">
         <v>20</v>
       </c>
@@ -7711,7 +7715,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="15.75" customHeight="1">
+    <row r="94" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A94" s="10">
         <v>24</v>
       </c>
@@ -7725,7 +7729,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="15.75" customHeight="1">
+    <row r="95" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A95" s="10">
         <v>28</v>
       </c>
@@ -7739,7 +7743,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="15.75" customHeight="1">
+    <row r="96" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A96" s="10">
         <v>32</v>
       </c>
@@ -7753,7 +7757,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="15.75" customHeight="1">
+    <row r="97" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A97" s="10">
         <v>6</v>
       </c>
@@ -7770,7 +7774,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="15.75" customHeight="1">
+    <row r="98" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A98" s="10">
         <v>28</v>
       </c>
@@ -7787,7 +7791,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="15.75" customHeight="1">
+    <row r="99" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A99" s="10">
         <v>28</v>
       </c>
@@ -7804,7 +7808,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="15.75" customHeight="1">
+    <row r="100" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A100" s="10">
         <v>28</v>
       </c>
@@ -7832,10 +7836,10 @@
         <v>14</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" ht="15.75" customHeight="1">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A102" s="10">
         <v>32</v>
       </c>
@@ -7849,7 +7853,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="15.75" customHeight="1">
+    <row r="103" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A103" s="10">
         <v>32</v>
       </c>
@@ -7863,7 +7867,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="15.75" customHeight="1">
+    <row r="104" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A104" s="10">
         <v>32</v>
       </c>
@@ -7877,7 +7881,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="15.75" customHeight="1">
+    <row r="105" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A105" s="10">
         <v>32</v>
       </c>
@@ -7891,7 +7895,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="15.75" customHeight="1">
+    <row r="106" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A106" s="10">
         <v>32</v>
       </c>
@@ -7905,7 +7909,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="15.75" customHeight="1">
+    <row r="107" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A107" s="10">
         <v>32</v>
       </c>
@@ -7919,7 +7923,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="15.75" customHeight="1">
+    <row r="108" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A108" s="10">
         <v>32</v>
       </c>
@@ -7933,7 +7937,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="15.75" customHeight="1">
+    <row r="109" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A109" s="10">
         <v>28</v>
       </c>
@@ -7947,7 +7951,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="15.75" customHeight="1">
+    <row r="110" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A110" s="10">
         <v>28</v>
       </c>
@@ -7961,7 +7965,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="15.75" customHeight="1">
+    <row r="111" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A111" s="10">
         <v>28</v>
       </c>
@@ -7975,7 +7979,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="15.75" customHeight="1">
+    <row r="112" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A112" s="10">
         <v>24</v>
       </c>
@@ -7989,7 +7993,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="15.75" customHeight="1">
+    <row r="113" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A113" s="10">
         <v>24</v>
       </c>
@@ -8003,7 +8007,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="15.75" customHeight="1">
+    <row r="114" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A114" s="10">
         <v>24</v>
       </c>
@@ -8017,7 +8021,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="15.75" customHeight="1">
+    <row r="115" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A115" s="10">
         <v>20</v>
       </c>
@@ -8031,7 +8035,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="15.75" customHeight="1">
+    <row r="116" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A116" s="10">
         <v>20</v>
       </c>
@@ -8045,7 +8049,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="15.75" customHeight="1">
+    <row r="117" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A117" s="10">
         <v>20</v>
       </c>
@@ -8059,7 +8063,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="15.75" customHeight="1">
+    <row r="118" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A118" s="10">
         <v>16</v>
       </c>
@@ -8073,7 +8077,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="15.75" customHeight="1">
+    <row r="119" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A119" s="10">
         <v>16</v>
       </c>
@@ -8087,7 +8091,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="15.75" customHeight="1">
+    <row r="120" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A120" s="10">
         <v>16</v>
       </c>
@@ -8101,7 +8105,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="15.75" customHeight="1">
+    <row r="121" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A121" s="10">
         <v>12</v>
       </c>
@@ -8115,7 +8119,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="15.75" customHeight="1">
+    <row r="122" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A122" s="10">
         <v>12</v>
       </c>
@@ -8129,7 +8133,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="15.75" customHeight="1">
+    <row r="123" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A123" s="10">
         <v>12</v>
       </c>
@@ -8143,7 +8147,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="15.75" customHeight="1">
+    <row r="124" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A124" s="10">
         <v>8</v>
       </c>
@@ -8157,7 +8161,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="15.75" customHeight="1">
+    <row r="125" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A125" s="10">
         <v>8</v>
       </c>
@@ -8171,7 +8175,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="15.75" customHeight="1">
+    <row r="126" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A126" s="10">
         <v>8</v>
       </c>
@@ -8185,7 +8189,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="15.75" customHeight="1">
+    <row r="127" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A127" s="10">
         <v>4</v>
       </c>
@@ -8199,7 +8203,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="15.75" customHeight="1">
+    <row r="128" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A128" s="10">
         <v>4</v>
       </c>
@@ -8213,7 +8217,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="15.75" customHeight="1">
+    <row r="129" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A129" s="10">
         <v>4</v>
       </c>
@@ -8227,7 +8231,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="15.75" customHeight="1">
+    <row r="130" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A130" s="10">
         <v>1</v>
       </c>
@@ -8241,7 +8245,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="15.75" customHeight="1">
+    <row r="131" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A131" s="10">
         <v>1</v>
       </c>
@@ -8255,7 +8259,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="15.75" customHeight="1">
+    <row r="132" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A132" s="10">
         <v>1</v>
       </c>
@@ -8269,7 +8273,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="15.75" customHeight="1">
+    <row r="133" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A133" s="10">
         <v>4</v>
       </c>
@@ -8283,7 +8287,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="15.75" customHeight="1">
+    <row r="134" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A134" s="10">
         <v>20</v>
       </c>
@@ -8297,7 +8301,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="15.75" customHeight="1">
+    <row r="135" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A135" s="10">
         <v>28</v>
       </c>
@@ -8311,7 +8315,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="15.75" customHeight="1">
+    <row r="136" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A136" s="10">
         <v>8</v>
       </c>
@@ -8328,7 +8332,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="15.75" customHeight="1">
+    <row r="137" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A137" s="10">
         <v>8</v>
       </c>
@@ -8345,7 +8349,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="15.75" customHeight="1">
+    <row r="138" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A138" s="10">
         <v>8</v>
       </c>
@@ -8362,7 +8366,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="15.75" customHeight="1">
+    <row r="139" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A139" s="10">
         <v>8</v>
       </c>
@@ -8379,7 +8383,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="15.75" customHeight="1">
+    <row r="140" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A140" s="10">
         <v>8</v>
       </c>
@@ -8396,7 +8400,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="15.75" customHeight="1">
+    <row r="141" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A141" s="10">
         <v>18</v>
       </c>
@@ -8413,7 +8417,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="15.75" customHeight="1">
+    <row r="142" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A142" s="10">
         <v>18</v>
       </c>
@@ -8430,7 +8434,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="15.75" customHeight="1">
+    <row r="143" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A143" s="10">
         <v>18</v>
       </c>
@@ -8447,7 +8451,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="15.75" customHeight="1">
+    <row r="144" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A144" s="10">
         <v>18</v>
       </c>
@@ -8464,7 +8468,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="15.75" customHeight="1">
+    <row r="145" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A145" s="10">
         <v>20</v>
       </c>
@@ -8484,7 +8488,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="15.75" customHeight="1">
+    <row r="146" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A146" s="10">
         <v>28</v>
       </c>
@@ -8504,7 +8508,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="15.75" customHeight="1">
+    <row r="147" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A147" s="10">
         <v>30</v>
       </c>
@@ -8521,7 +8525,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="15.75" customHeight="1">
+    <row r="148" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A148" s="10">
         <v>30</v>
       </c>
@@ -8538,7 +8542,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="15.75" customHeight="1">
+    <row r="149" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A149" s="10">
         <v>30</v>
       </c>
@@ -8558,7 +8562,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="15.75" customHeight="1">
+    <row r="150" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A150" s="10">
         <v>30</v>
       </c>
@@ -8575,7 +8579,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="15.75" customHeight="1">
+    <row r="151" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A151" s="10">
         <v>30</v>
       </c>
@@ -8592,7 +8596,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="15.75" customHeight="1">
+    <row r="152" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A152" s="10">
         <v>30</v>
       </c>
@@ -8609,7 +8613,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="15.75" customHeight="1">
+    <row r="153" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A153" s="10">
         <v>32</v>
       </c>
@@ -8626,7 +8630,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="15.75" customHeight="1">
+    <row r="154" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A154" s="10">
         <v>32</v>
       </c>
@@ -8643,7 +8647,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="15.75" customHeight="1">
+    <row r="155" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A155" s="10">
         <v>32</v>
       </c>
@@ -8660,7 +8664,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="15.75" customHeight="1">
+    <row r="156" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A156" s="10">
         <v>32</v>
       </c>
@@ -8677,7 +8681,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="15.75" customHeight="1">
+    <row r="157" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A157" s="10">
         <v>1</v>
       </c>
@@ -8694,7 +8698,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="15.75" customHeight="1">
+    <row r="158" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A158" s="10">
         <v>4</v>
       </c>
@@ -8711,7 +8715,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="15.75" customHeight="1">
+    <row r="159" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A159" s="10">
         <v>8</v>
       </c>
@@ -8728,7 +8732,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="15.75" customHeight="1">
+    <row r="160" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A160" s="10">
         <v>12</v>
       </c>
@@ -8745,7 +8749,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="15.75" customHeight="1">
+    <row r="161" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A161" s="10">
         <v>16</v>
       </c>
@@ -8762,7 +8766,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="15.75" customHeight="1">
+    <row r="162" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A162" s="10">
         <v>20</v>
       </c>
@@ -8779,7 +8783,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="163" spans="1:5" ht="15.75" customHeight="1">
+    <row r="163" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A163" s="10">
         <v>24</v>
       </c>
@@ -8796,7 +8800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="164" spans="1:5" ht="15.75" customHeight="1">
+    <row r="164" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A164" s="10">
         <v>28</v>
       </c>
@@ -9656,7 +9660,13 @@
     <row r="1005" ht="15.75" customHeight="1"/>
     <row r="1006" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="A1:E164" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:E164" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Natural Armor"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bonus type on Sapphire of Natural Armor augment to be a Natural bonus to AC to match other affixes (#86)
Co-authored-by: joenuts <>
</commit_message>
<xml_diff>
--- a/data-builder/augments.xlsx
+++ b/data-builder/augments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E644CA-7796-4CA0-BFFF-D64F4D48B3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED03EE9-B1A8-4545-A57E-EB9B9E7C15AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19500" yWindow="10830" windowWidth="24150" windowHeight="18330" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="32040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Yellow" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="410">
   <si>
     <t>Minimum Level</t>
   </si>
@@ -1275,6 +1275,9 @@
   </si>
   <si>
     <t>Deflection</t>
+  </si>
+  <si>
+    <t>Natural</t>
   </si>
 </sst>
 </file>
@@ -1282,7 +1285,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -1372,10 +1375,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6387,10 +6390,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A164"/>
+      <selection activeCell="E165" sqref="E165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -6434,10 +6438,10 @@
         <v>1</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" hidden="1">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -6451,7 +6455,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" hidden="1">
       <c r="A4" s="10">
         <v>1</v>
       </c>
@@ -6465,7 +6469,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" hidden="1">
       <c r="A5" s="10">
         <v>1</v>
       </c>
@@ -6479,7 +6483,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" hidden="1">
       <c r="A6" s="10">
         <v>1</v>
       </c>
@@ -6493,7 +6497,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" hidden="1">
       <c r="A7" s="10">
         <v>1</v>
       </c>
@@ -6518,10 +6522,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" hidden="1">
       <c r="A9" s="10">
         <v>4</v>
       </c>
@@ -6535,7 +6539,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" hidden="1">
       <c r="A10" s="10">
         <v>4</v>
       </c>
@@ -6549,7 +6553,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" hidden="1">
       <c r="A11" s="10">
         <v>4</v>
       </c>
@@ -6563,7 +6567,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" hidden="1">
       <c r="A12" s="10">
         <v>4</v>
       </c>
@@ -6577,7 +6581,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" hidden="1">
       <c r="A13" s="10">
         <v>4</v>
       </c>
@@ -6602,10 +6606,10 @@
         <v>5</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" hidden="1">
       <c r="A15" s="10">
         <v>8</v>
       </c>
@@ -6619,7 +6623,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" hidden="1">
       <c r="A16" s="10">
         <v>8</v>
       </c>
@@ -6633,7 +6637,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" hidden="1">
       <c r="A17" s="10">
         <v>8</v>
       </c>
@@ -6647,7 +6651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" hidden="1">
       <c r="A18" s="10">
         <v>8</v>
       </c>
@@ -6661,7 +6665,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" hidden="1">
       <c r="A19" s="10">
         <v>8</v>
       </c>
@@ -6686,10 +6690,10 @@
         <v>6</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A21" s="10">
         <v>12</v>
       </c>
@@ -6703,7 +6707,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1">
+    <row r="22" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A22" s="10">
         <v>12</v>
       </c>
@@ -6717,7 +6721,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1">
+    <row r="23" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A23" s="10">
         <v>12</v>
       </c>
@@ -6731,7 +6735,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1">
+    <row r="24" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A24" s="10">
         <v>12</v>
       </c>
@@ -6745,7 +6749,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1">
+    <row r="25" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A25" s="10">
         <v>12</v>
       </c>
@@ -6770,10 +6774,10 @@
         <v>8</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A27" s="10">
         <v>16</v>
       </c>
@@ -6787,7 +6791,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+    <row r="28" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A28" s="10">
         <v>16</v>
       </c>
@@ -6801,7 +6805,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1">
+    <row r="29" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A29" s="10">
         <v>16</v>
       </c>
@@ -6815,7 +6819,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+    <row r="30" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A30" s="10">
         <v>16</v>
       </c>
@@ -6840,10 +6844,10 @@
         <v>9</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A32" s="10">
         <v>20</v>
       </c>
@@ -6857,7 +6861,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1">
+    <row r="33" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A33" s="10">
         <v>20</v>
       </c>
@@ -6871,7 +6875,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1">
+    <row r="34" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A34" s="10">
         <v>20</v>
       </c>
@@ -6885,7 +6889,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1">
+    <row r="35" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A35" s="10">
         <v>20</v>
       </c>
@@ -6899,7 +6903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1">
+    <row r="36" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A36" s="10">
         <v>20</v>
       </c>
@@ -6924,10 +6928,10 @@
         <v>11</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A38" s="10">
         <v>24</v>
       </c>
@@ -6941,7 +6945,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1">
+    <row r="39" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A39" s="10">
         <v>24</v>
       </c>
@@ -6955,7 +6959,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1">
+    <row r="40" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A40" s="10">
         <v>24</v>
       </c>
@@ -6969,7 +6973,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1">
+    <row r="41" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A41" s="10">
         <v>24</v>
       </c>
@@ -6994,10 +6998,10 @@
         <v>12</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A43" s="10">
         <v>28</v>
       </c>
@@ -7011,7 +7015,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1">
+    <row r="44" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A44" s="10">
         <v>28</v>
       </c>
@@ -7025,7 +7029,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1">
+    <row r="45" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A45" s="10">
         <v>28</v>
       </c>
@@ -7039,7 +7043,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1">
+    <row r="46" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A46" s="10">
         <v>28</v>
       </c>
@@ -7053,7 +7057,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1">
+    <row r="47" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A47" s="10">
         <v>12</v>
       </c>
@@ -7067,7 +7071,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1">
+    <row r="48" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A48" s="10">
         <v>16</v>
       </c>
@@ -7081,7 +7085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1">
+    <row r="49" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A49" s="10">
         <v>20</v>
       </c>
@@ -7095,7 +7099,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1">
+    <row r="50" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A50" s="10">
         <v>12</v>
       </c>
@@ -7109,7 +7113,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1">
+    <row r="51" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A51" s="10">
         <v>20</v>
       </c>
@@ -7123,7 +7127,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1">
+    <row r="52" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A52" s="10">
         <v>1</v>
       </c>
@@ -7137,7 +7141,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1">
+    <row r="53" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A53" s="10">
         <v>4</v>
       </c>
@@ -7151,7 +7155,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1">
+    <row r="54" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A54" s="10">
         <v>8</v>
       </c>
@@ -7165,7 +7169,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15.75" customHeight="1">
+    <row r="55" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A55" s="10">
         <v>12</v>
       </c>
@@ -7179,7 +7183,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15.75" customHeight="1">
+    <row r="56" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A56" s="10">
         <v>16</v>
       </c>
@@ -7193,7 +7197,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="15.75" customHeight="1">
+    <row r="57" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A57" s="10">
         <v>20</v>
       </c>
@@ -7207,7 +7211,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15.75" customHeight="1">
+    <row r="58" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A58" s="10">
         <v>24</v>
       </c>
@@ -7221,7 +7225,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15.75" customHeight="1">
+    <row r="59" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A59" s="10">
         <v>28</v>
       </c>
@@ -7235,7 +7239,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="15.75" customHeight="1">
+    <row r="60" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A60" s="10">
         <v>32</v>
       </c>
@@ -7249,7 +7253,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1">
+    <row r="61" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A61" s="10">
         <v>1</v>
       </c>
@@ -7263,7 +7267,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1">
+    <row r="62" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A62" s="10">
         <v>4</v>
       </c>
@@ -7277,7 +7281,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1">
+    <row r="63" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A63" s="10">
         <v>8</v>
       </c>
@@ -7291,7 +7295,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1">
+    <row r="64" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A64" s="10">
         <v>12</v>
       </c>
@@ -7305,7 +7309,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1">
+    <row r="65" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A65" s="10">
         <v>16</v>
       </c>
@@ -7319,7 +7323,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1">
+    <row r="66" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A66" s="10">
         <v>20</v>
       </c>
@@ -7333,7 +7337,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1">
+    <row r="67" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A67" s="10">
         <v>24</v>
       </c>
@@ -7347,7 +7351,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1">
+    <row r="68" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A68" s="10">
         <v>28</v>
       </c>
@@ -7361,7 +7365,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1">
+    <row r="69" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A69" s="10">
         <v>32</v>
       </c>
@@ -7375,7 +7379,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1">
+    <row r="70" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A70" s="10">
         <v>1</v>
       </c>
@@ -7389,7 +7393,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1">
+    <row r="71" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A71" s="10">
         <v>4</v>
       </c>
@@ -7403,7 +7407,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1">
+    <row r="72" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A72" s="10">
         <v>8</v>
       </c>
@@ -7417,7 +7421,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1">
+    <row r="73" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A73" s="10">
         <v>12</v>
       </c>
@@ -7431,7 +7435,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1">
+    <row r="74" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A74" s="10">
         <v>16</v>
       </c>
@@ -7445,7 +7449,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1">
+    <row r="75" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A75" s="10">
         <v>20</v>
       </c>
@@ -7459,7 +7463,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1">
+    <row r="76" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A76" s="10">
         <v>24</v>
       </c>
@@ -7473,7 +7477,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1">
+    <row r="77" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A77" s="10">
         <v>28</v>
       </c>
@@ -7487,7 +7491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1">
+    <row r="78" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A78" s="10">
         <v>32</v>
       </c>
@@ -7501,7 +7505,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1">
+    <row r="79" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A79" s="10">
         <v>1</v>
       </c>
@@ -7515,7 +7519,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1">
+    <row r="80" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A80" s="10">
         <v>4</v>
       </c>
@@ -7529,7 +7533,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1">
+    <row r="81" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A81" s="10">
         <v>8</v>
       </c>
@@ -7543,7 +7547,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1">
+    <row r="82" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A82" s="10">
         <v>12</v>
       </c>
@@ -7557,7 +7561,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1">
+    <row r="83" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A83" s="10">
         <v>16</v>
       </c>
@@ -7571,7 +7575,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="15.75" customHeight="1">
+    <row r="84" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A84" s="10">
         <v>20</v>
       </c>
@@ -7585,7 +7589,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="15.75" customHeight="1">
+    <row r="85" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A85" s="10">
         <v>24</v>
       </c>
@@ -7599,7 +7603,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="15.75" customHeight="1">
+    <row r="86" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A86" s="10">
         <v>28</v>
       </c>
@@ -7613,7 +7617,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="15.75" customHeight="1">
+    <row r="87" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A87" s="10">
         <v>32</v>
       </c>
@@ -7627,7 +7631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="15.75" customHeight="1">
+    <row r="88" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A88" s="10">
         <v>1</v>
       </c>
@@ -7641,7 +7645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="15.75" customHeight="1">
+    <row r="89" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A89" s="10">
         <v>4</v>
       </c>
@@ -7655,7 +7659,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="15.75" customHeight="1">
+    <row r="90" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A90" s="10">
         <v>8</v>
       </c>
@@ -7669,7 +7673,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="15.75" customHeight="1">
+    <row r="91" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A91" s="10">
         <v>12</v>
       </c>
@@ -7683,7 +7687,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="15.75" customHeight="1">
+    <row r="92" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A92" s="10">
         <v>16</v>
       </c>
@@ -7697,7 +7701,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="15.75" customHeight="1">
+    <row r="93" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A93" s="10">
         <v>20</v>
       </c>
@@ -7711,7 +7715,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="15.75" customHeight="1">
+    <row r="94" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A94" s="10">
         <v>24</v>
       </c>
@@ -7725,7 +7729,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="15.75" customHeight="1">
+    <row r="95" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A95" s="10">
         <v>28</v>
       </c>
@@ -7739,7 +7743,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="15.75" customHeight="1">
+    <row r="96" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A96" s="10">
         <v>32</v>
       </c>
@@ -7753,7 +7757,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="15.75" customHeight="1">
+    <row r="97" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A97" s="10">
         <v>6</v>
       </c>
@@ -7770,7 +7774,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="15.75" customHeight="1">
+    <row r="98" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A98" s="10">
         <v>28</v>
       </c>
@@ -7787,7 +7791,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="15.75" customHeight="1">
+    <row r="99" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A99" s="10">
         <v>28</v>
       </c>
@@ -7804,7 +7808,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="15.75" customHeight="1">
+    <row r="100" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A100" s="10">
         <v>28</v>
       </c>
@@ -7832,10 +7836,10 @@
         <v>14</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" ht="15.75" customHeight="1">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A102" s="10">
         <v>32</v>
       </c>
@@ -7849,7 +7853,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="15.75" customHeight="1">
+    <row r="103" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A103" s="10">
         <v>32</v>
       </c>
@@ -7863,7 +7867,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="15.75" customHeight="1">
+    <row r="104" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A104" s="10">
         <v>32</v>
       </c>
@@ -7877,7 +7881,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="15.75" customHeight="1">
+    <row r="105" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A105" s="10">
         <v>32</v>
       </c>
@@ -7891,7 +7895,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="15.75" customHeight="1">
+    <row r="106" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A106" s="10">
         <v>32</v>
       </c>
@@ -7905,7 +7909,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="15.75" customHeight="1">
+    <row r="107" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A107" s="10">
         <v>32</v>
       </c>
@@ -7919,7 +7923,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="15.75" customHeight="1">
+    <row r="108" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A108" s="10">
         <v>32</v>
       </c>
@@ -7933,7 +7937,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="15.75" customHeight="1">
+    <row r="109" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A109" s="10">
         <v>28</v>
       </c>
@@ -7947,7 +7951,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="15.75" customHeight="1">
+    <row r="110" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A110" s="10">
         <v>28</v>
       </c>
@@ -7961,7 +7965,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="15.75" customHeight="1">
+    <row r="111" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A111" s="10">
         <v>28</v>
       </c>
@@ -7975,7 +7979,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="15.75" customHeight="1">
+    <row r="112" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A112" s="10">
         <v>24</v>
       </c>
@@ -7989,7 +7993,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="15.75" customHeight="1">
+    <row r="113" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A113" s="10">
         <v>24</v>
       </c>
@@ -8003,7 +8007,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="15.75" customHeight="1">
+    <row r="114" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A114" s="10">
         <v>24</v>
       </c>
@@ -8017,7 +8021,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="15.75" customHeight="1">
+    <row r="115" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A115" s="10">
         <v>20</v>
       </c>
@@ -8031,7 +8035,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="15.75" customHeight="1">
+    <row r="116" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A116" s="10">
         <v>20</v>
       </c>
@@ -8045,7 +8049,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="15.75" customHeight="1">
+    <row r="117" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A117" s="10">
         <v>20</v>
       </c>
@@ -8059,7 +8063,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="15.75" customHeight="1">
+    <row r="118" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A118" s="10">
         <v>16</v>
       </c>
@@ -8073,7 +8077,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="15.75" customHeight="1">
+    <row r="119" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A119" s="10">
         <v>16</v>
       </c>
@@ -8087,7 +8091,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="15.75" customHeight="1">
+    <row r="120" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A120" s="10">
         <v>16</v>
       </c>
@@ -8101,7 +8105,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="15.75" customHeight="1">
+    <row r="121" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A121" s="10">
         <v>12</v>
       </c>
@@ -8115,7 +8119,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="15.75" customHeight="1">
+    <row r="122" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A122" s="10">
         <v>12</v>
       </c>
@@ -8129,7 +8133,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="15.75" customHeight="1">
+    <row r="123" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A123" s="10">
         <v>12</v>
       </c>
@@ -8143,7 +8147,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="15.75" customHeight="1">
+    <row r="124" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A124" s="10">
         <v>8</v>
       </c>
@@ -8157,7 +8161,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="15.75" customHeight="1">
+    <row r="125" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A125" s="10">
         <v>8</v>
       </c>
@@ -8171,7 +8175,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="15.75" customHeight="1">
+    <row r="126" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A126" s="10">
         <v>8</v>
       </c>
@@ -8185,7 +8189,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="15.75" customHeight="1">
+    <row r="127" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A127" s="10">
         <v>4</v>
       </c>
@@ -8199,7 +8203,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="15.75" customHeight="1">
+    <row r="128" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A128" s="10">
         <v>4</v>
       </c>
@@ -8213,7 +8217,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="15.75" customHeight="1">
+    <row r="129" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A129" s="10">
         <v>4</v>
       </c>
@@ -8227,7 +8231,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="15.75" customHeight="1">
+    <row r="130" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A130" s="10">
         <v>1</v>
       </c>
@@ -8241,7 +8245,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="15.75" customHeight="1">
+    <row r="131" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A131" s="10">
         <v>1</v>
       </c>
@@ -8255,7 +8259,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="15.75" customHeight="1">
+    <row r="132" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A132" s="10">
         <v>1</v>
       </c>
@@ -8269,7 +8273,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="15.75" customHeight="1">
+    <row r="133" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A133" s="10">
         <v>4</v>
       </c>
@@ -8283,7 +8287,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="15.75" customHeight="1">
+    <row r="134" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A134" s="10">
         <v>20</v>
       </c>
@@ -8297,7 +8301,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="15.75" customHeight="1">
+    <row r="135" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A135" s="10">
         <v>28</v>
       </c>
@@ -8311,7 +8315,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="15.75" customHeight="1">
+    <row r="136" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A136" s="10">
         <v>8</v>
       </c>
@@ -8328,7 +8332,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="15.75" customHeight="1">
+    <row r="137" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A137" s="10">
         <v>8</v>
       </c>
@@ -8345,7 +8349,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="15.75" customHeight="1">
+    <row r="138" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A138" s="10">
         <v>8</v>
       </c>
@@ -8362,7 +8366,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="15.75" customHeight="1">
+    <row r="139" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A139" s="10">
         <v>8</v>
       </c>
@@ -8379,7 +8383,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="15.75" customHeight="1">
+    <row r="140" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A140" s="10">
         <v>8</v>
       </c>
@@ -8396,7 +8400,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="15.75" customHeight="1">
+    <row r="141" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A141" s="10">
         <v>18</v>
       </c>
@@ -8413,7 +8417,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="15.75" customHeight="1">
+    <row r="142" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A142" s="10">
         <v>18</v>
       </c>
@@ -8430,7 +8434,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="15.75" customHeight="1">
+    <row r="143" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A143" s="10">
         <v>18</v>
       </c>
@@ -8447,7 +8451,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="15.75" customHeight="1">
+    <row r="144" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A144" s="10">
         <v>18</v>
       </c>
@@ -8464,7 +8468,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="15.75" customHeight="1">
+    <row r="145" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A145" s="10">
         <v>20</v>
       </c>
@@ -8484,7 +8488,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="15.75" customHeight="1">
+    <row r="146" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A146" s="10">
         <v>28</v>
       </c>
@@ -8504,7 +8508,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="15.75" customHeight="1">
+    <row r="147" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A147" s="10">
         <v>30</v>
       </c>
@@ -8521,7 +8525,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="15.75" customHeight="1">
+    <row r="148" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A148" s="10">
         <v>30</v>
       </c>
@@ -8538,7 +8542,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="15.75" customHeight="1">
+    <row r="149" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A149" s="10">
         <v>30</v>
       </c>
@@ -8558,7 +8562,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="15.75" customHeight="1">
+    <row r="150" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A150" s="10">
         <v>30</v>
       </c>
@@ -8575,7 +8579,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="15.75" customHeight="1">
+    <row r="151" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A151" s="10">
         <v>30</v>
       </c>
@@ -8592,7 +8596,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="15.75" customHeight="1">
+    <row r="152" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A152" s="10">
         <v>30</v>
       </c>
@@ -8609,7 +8613,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="15.75" customHeight="1">
+    <row r="153" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A153" s="10">
         <v>32</v>
       </c>
@@ -8626,7 +8630,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="15.75" customHeight="1">
+    <row r="154" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A154" s="10">
         <v>32</v>
       </c>
@@ -8643,7 +8647,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="15.75" customHeight="1">
+    <row r="155" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A155" s="10">
         <v>32</v>
       </c>
@@ -8660,7 +8664,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="15.75" customHeight="1">
+    <row r="156" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A156" s="10">
         <v>32</v>
       </c>
@@ -8677,7 +8681,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="15.75" customHeight="1">
+    <row r="157" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A157" s="10">
         <v>1</v>
       </c>
@@ -8694,7 +8698,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="15.75" customHeight="1">
+    <row r="158" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A158" s="10">
         <v>4</v>
       </c>
@@ -8711,7 +8715,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="15.75" customHeight="1">
+    <row r="159" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A159" s="10">
         <v>8</v>
       </c>
@@ -8728,7 +8732,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="15.75" customHeight="1">
+    <row r="160" spans="1:6" ht="15.75" hidden="1" customHeight="1">
       <c r="A160" s="10">
         <v>12</v>
       </c>
@@ -8745,7 +8749,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="15.75" customHeight="1">
+    <row r="161" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A161" s="10">
         <v>16</v>
       </c>
@@ -8762,7 +8766,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="15.75" customHeight="1">
+    <row r="162" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A162" s="10">
         <v>20</v>
       </c>
@@ -8779,7 +8783,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="163" spans="1:5" ht="15.75" customHeight="1">
+    <row r="163" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A163" s="10">
         <v>24</v>
       </c>
@@ -8796,7 +8800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="164" spans="1:5" ht="15.75" customHeight="1">
+    <row r="164" spans="1:5" ht="15.75" hidden="1" customHeight="1">
       <c r="A164" s="10">
         <v>28</v>
       </c>
@@ -9656,7 +9660,13 @@
     <row r="1005" ht="15.75" customHeight="1"/>
     <row r="1006" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="A1:E164" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:E164" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Natural Armor"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>